<commit_message>
Suppress annoying xlrd warning "WARNING *** file size ..." #37 Add specific code for merging Audubon results files #38 Convert downloads from Audubon results page to Single format #34
</commit_message>
<xml_diff>
--- a/parameters/Local/LocalTranslations.xlsx
+++ b/parameters/Local/LocalTranslations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/CBCPipeline/parameters-others/ParseSpeciesPDFs/Local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/automatingcbc/parameters/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DEB2FD-764A-784B-8FC6-73258B1C39D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD29CB-0566-D442-B341-22066ED0044F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23420" yWindow="4600" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23400" yWindow="4580" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Possible Translations" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="692">
   <si>
     <t>LocalSpeciesName</t>
   </si>
@@ -2094,6 +2094,21 @@
   </si>
   <si>
     <t>Goldfinch sp.</t>
+  </si>
+  <si>
+    <t>Mallard x American Black Duck (hybrid)</t>
+  </si>
+  <si>
+    <t>american black duck x mallard (hybrid)</t>
+  </si>
+  <si>
+    <t>le conte's sparrow</t>
+  </si>
+  <si>
+    <t>TXMM</t>
+  </si>
+  <si>
+    <t>LeConte's sparrow</t>
   </si>
 </sst>
 </file>
@@ -2348,8 +2363,8 @@
     <tableColumn id="23" xr3:uid="{BB3F355D-235C-4542-926A-95E31CE2B62E}" name="levd"/>
     <tableColumn id="21" xr3:uid="{D5C2681A-1D9D-304C-A87E-BE29C276C2FC}" name="match_whole_line"/>
     <tableColumn id="22" xr3:uid="{C8B2D0A9-713C-3F4B-A9D3-3AB173A85E52}" name="regex"/>
-    <tableColumn id="20" xr3:uid="{A8843416-1456-EE4D-A56B-05466967065E}" name="circle" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{A7870F45-FD68-A34A-931C-8E73DD227839}" name="comments" dataDxfId="0"/>
+    <tableColumn id="20" xr3:uid="{A8843416-1456-EE4D-A56B-05466967065E}" name="circle" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{A7870F45-FD68-A34A-931C-8E73DD227839}" name="comments" dataDxfId="2"/>
     <tableColumn id="26" xr3:uid="{BCD504FC-6B5A-2F4A-9C73-0D4A0F0CAF44}" name="AltName1"/>
     <tableColumn id="27" xr3:uid="{90D8A827-36BA-6B4C-8D6B-E8C1D5CC0A9E}" name="lev1"/>
     <tableColumn id="28" xr3:uid="{2C3BD86A-E04B-7549-AA82-472AAD31C35E}" name="AltName2"/>
@@ -2378,10 +2393,10 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="eBirdSpeciesName"/>
     <tableColumn id="21" xr3:uid="{936EC4A6-EE3A-494F-A432-F5C4587CB081}" name="match_whole_line"/>
     <tableColumn id="22" xr3:uid="{29F377A7-C014-8F4C-841A-9D6572D667EE}" name="regex"/>
-    <tableColumn id="20" xr3:uid="{822943D7-8619-E140-8C43-A6388430313E}" name="circle" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{822943D7-8619-E140-8C43-A6388430313E}" name="circle" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rare"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Hybrid"/>
-    <tableColumn id="24" xr3:uid="{4A34E1B2-BC28-F242-8B86-D3CE5C67D30C}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{4A34E1B2-BC28-F242-8B86-D3CE5C67D30C}" name="Comments" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AltName1"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="AltName2"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="AltName3"/>
@@ -2723,10 +2738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080E692E-9BC3-734D-8C24-67E54468B45D}">
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6251,6 +6267,40 @@
       </c>
       <c r="F159" s="1" t="s">
         <v>672</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" t="s">
+        <v>688</v>
+      </c>
+      <c r="B160" t="s">
+        <v>687</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
+        <v>689</v>
+      </c>
+      <c r="B161" t="s">
+        <v>691</v>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+      <c r="E161" t="b">
+        <v>0</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
don't strip out Feral, will fail to process Rock Pigeon (Feral) properly
</commit_message>
<xml_diff>
--- a/parameters/Local/LocalTranslations.xlsx
+++ b/parameters/Local/LocalTranslations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/automatingcbc/parameters/Local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/CBCPipeline/parameters/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD29CB-0566-D442-B341-22066ED0044F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71394D-E27E-6D4E-933D-A41ABFD259FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23400" yWindow="4580" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23420" yWindow="4600" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Possible Translations" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="688">
   <si>
     <t>LocalSpeciesName</t>
   </si>
@@ -2096,19 +2096,7 @@
     <t>Goldfinch sp.</t>
   </si>
   <si>
-    <t>Mallard x American Black Duck (hybrid)</t>
-  </si>
-  <si>
-    <t>american black duck x mallard (hybrid)</t>
-  </si>
-  <si>
-    <t>le conte's sparrow</t>
-  </si>
-  <si>
-    <t>TXMM</t>
-  </si>
-  <si>
-    <t>LeConte's sparrow</t>
+    <t>\b(cw|rare|immature|adult|ad|imm|juv|unknown age|exotic|subadult|unknown|mature)\b</t>
   </si>
 </sst>
 </file>
@@ -2738,11 +2726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080E692E-9BC3-734D-8C24-67E54468B45D}">
-  <dimension ref="A1:Q161"/>
+  <dimension ref="A1:Q159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4588,7 +4575,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="16" t="s">
-        <v>425</v>
+        <v>687</v>
       </c>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -6267,40 +6254,6 @@
       </c>
       <c r="F159" s="1" t="s">
         <v>672</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7">
-      <c r="A160" t="s">
-        <v>688</v>
-      </c>
-      <c r="B160" t="s">
-        <v>687</v>
-      </c>
-      <c r="D160" t="b">
-        <v>1</v>
-      </c>
-      <c r="E160" t="b">
-        <v>0</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161" t="s">
-        <v>689</v>
-      </c>
-      <c r="B161" t="s">
-        <v>691</v>
-      </c>
-      <c r="D161" t="b">
-        <v>1</v>
-      </c>
-      <c r="E161" t="b">
-        <v>0</v>
-      </c>
-      <c r="F161" s="1" t="s">
-        <v>690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add files for CAMH additional translations for CASJ
</commit_message>
<xml_diff>
--- a/parameters/Local/LocalTranslations.xlsx
+++ b/parameters/Local/LocalTranslations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/CBCPipeline/parameters/Local/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/automatingcbc/parameters/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71394D-E27E-6D4E-933D-A41ABFD259FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251A04E-EA00-0243-B123-BFB2311B629F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23420" yWindow="4600" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21580" yWindow="840" windowWidth="32740" windowHeight="24880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Possible Translations" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="694">
   <si>
     <t>LocalSpeciesName</t>
   </si>
@@ -2097,13 +2097,31 @@
   </si>
   <si>
     <t>\b(cw|rare|immature|adult|ad|imm|juv|unknown age|exotic|subadult|unknown|mature)\b</t>
+  </si>
+  <si>
+    <t>greater white fronted goose</t>
+  </si>
+  <si>
+    <t>northern rough-wing swallow</t>
+  </si>
+  <si>
+    <t>northern rough-winged swallow</t>
+  </si>
+  <si>
+    <t>western x glaucous-winged gull</t>
+  </si>
+  <si>
+    <t>northern shoveler x blue-winged teal</t>
+  </si>
+  <si>
+    <t>Blue-winged Teal x Northern Shoveler (hybrid)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2141,6 +2159,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="ArialMT"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2231,7 +2255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2307,6 +2331,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2726,10 +2751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080E692E-9BC3-734D-8C24-67E54468B45D}">
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162:F163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6254,6 +6279,74 @@
       </c>
       <c r="F159" s="1" t="s">
         <v>672</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="16">
+      <c r="A160" s="41" t="s">
+        <v>688</v>
+      </c>
+      <c r="B160" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
+        <v>689</v>
+      </c>
+      <c r="B161" t="s">
+        <v>690</v>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+      <c r="E161" t="b">
+        <v>0</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
+        <v>691</v>
+      </c>
+      <c r="B162" t="s">
+        <v>109</v>
+      </c>
+      <c r="D162" t="b">
+        <v>1</v>
+      </c>
+      <c r="E162" t="b">
+        <v>0</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
+        <v>692</v>
+      </c>
+      <c r="B163" t="s">
+        <v>693</v>
+      </c>
+      <c r="D163" t="b">
+        <v>1</v>
+      </c>
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>